<commit_message>
added new 4mhz low profile crystal to bom, updated c1,c2 cap part numbers
</commit_message>
<xml_diff>
--- a/doc/ecg_bom_logic_board.xlsx
+++ b/doc/ecg_bom_logic_board.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14520"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="157">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -72,9 +72,6 @@
     <t>BOM Lines</t>
   </si>
   <si>
-    <t>SMT</t>
-  </si>
-  <si>
     <t>Number of Components</t>
   </si>
   <si>
@@ -156,15 +153,6 @@
     <t>CRYSTAL 32.768KHZ 12.5PF SMD</t>
   </si>
   <si>
-    <t>XC1260CT-ND</t>
-  </si>
-  <si>
-    <t>ECS-41-20-5PX-TR</t>
-  </si>
-  <si>
-    <t>CRYSTAL 4.096MHZ 20PF SMD</t>
-  </si>
-  <si>
     <t>CONN1</t>
   </si>
   <si>
@@ -174,9 +162,6 @@
     <t>C1, C2</t>
   </si>
   <si>
-    <t>Murata Electronics North America</t>
-  </si>
-  <si>
     <t>TDK Corporation</t>
   </si>
   <si>
@@ -243,18 +228,6 @@
     <t>ERJ-1GEF1003C</t>
   </si>
   <si>
-    <t>Beat v1.0</t>
-  </si>
-  <si>
-    <t>490-6067-1-ND</t>
-  </si>
-  <si>
-    <t>GJM0335C0J220GB01D</t>
-  </si>
-  <si>
-    <t>CAP CER 22PF 6.3V 2% NP0 0201</t>
-  </si>
-  <si>
     <t>399-8604-1-ND</t>
   </si>
   <si>
@@ -487,6 +460,36 @@
   </si>
   <si>
     <t>TVS ARRAY ESD/CDE PROT SLP1006P2</t>
+  </si>
+  <si>
+    <t>445-7073-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C0G1E200G030BG</t>
+  </si>
+  <si>
+    <t>CAP CER 20PF 25V 2% NP0 0201</t>
+  </si>
+  <si>
+    <t>XC1570-ND</t>
+  </si>
+  <si>
+    <t>ECS-40-20-4VX</t>
+  </si>
+  <si>
+    <t>CRYSTAL 4MHZ 20PF THRU</t>
+  </si>
+  <si>
+    <t>TP1,TP2,TP5,TP6,TP7,TP8,TP9,TP12</t>
+  </si>
+  <si>
+    <t>DO NOT PLACE</t>
+  </si>
+  <si>
+    <t>P1,P2,P3,P4,P6,P7</t>
+  </si>
+  <si>
+    <t>Beat v1.1</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,6 +581,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -615,7 +625,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -701,6 +711,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -1016,9 +1032,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
@@ -1037,7 +1055,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="12" t="s">
-        <v>74</v>
+        <v>156</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1095,22 +1113,22 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>12</v>
@@ -1128,22 +1146,22 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="E5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="F5" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>12</v>
@@ -1161,22 +1179,22 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="F6" s="26" t="s">
         <v>32</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>33</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>12</v>
@@ -1209,7 +1227,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>12</v>
@@ -1227,22 +1245,22 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="30" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>12</v>
@@ -1260,22 +1278,22 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="30" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>12</v>
@@ -1305,22 +1323,22 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="E11" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="F11" s="26" t="s">
         <v>43</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>44</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>12</v>
@@ -1338,22 +1356,22 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="F12" s="26" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>40</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>12</v>
@@ -1371,22 +1389,22 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>12</v>
@@ -1395,11 +1413,11 @@
         <v>1</v>
       </c>
       <c r="I13" s="23">
-        <v>0.64</v>
+        <v>1.78</v>
       </c>
       <c r="J13" s="23">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1416,22 +1434,22 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="30" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>12</v>
@@ -1449,22 +1467,22 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="30" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>12</v>
@@ -1482,22 +1500,22 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="30" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>12</v>
@@ -1527,22 +1545,22 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>75</v>
+        <v>147</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>77</v>
+        <v>149</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>12</v>
@@ -1551,31 +1569,31 @@
         <v>2</v>
       </c>
       <c r="I19" s="23">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="J19" s="23">
         <f t="shared" si="0"/>
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="30" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>12</v>
@@ -1593,22 +1611,22 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="30" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>12</v>
@@ -1626,22 +1644,22 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="30" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>12</v>
@@ -1659,22 +1677,22 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="30" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>12</v>
@@ -1692,22 +1710,22 @@
     </row>
     <row r="24" spans="1:12" s="5" customFormat="1">
       <c r="A24" s="30" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>12</v>
@@ -1726,22 +1744,22 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="30" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D25" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="26" t="s">
         <v>52</v>
-      </c>
-      <c r="E25" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>57</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>12</v>
@@ -1759,22 +1777,22 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="30" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>12</v>
@@ -1804,22 +1822,22 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="30" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>12</v>
@@ -1837,22 +1855,22 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="30" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F29" s="26" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>12</v>
@@ -1870,22 +1888,22 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="30" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>12</v>
@@ -1903,22 +1921,22 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="30" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>12</v>
@@ -1936,22 +1954,22 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="26" t="s">
         <v>65</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="F32" s="26" t="s">
-        <v>70</v>
       </c>
       <c r="G32" s="19" t="s">
         <v>12</v>
@@ -1969,22 +1987,22 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="30" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="G33" s="19" t="s">
         <v>12</v>
@@ -2002,22 +2020,22 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="30" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="G34" s="19" t="s">
         <v>12</v>
@@ -2035,22 +2053,22 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="30" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G35" s="19" t="s">
         <v>12</v>
@@ -2080,22 +2098,22 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="30" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="G37" s="19" t="s">
         <v>12</v>
@@ -2125,22 +2143,22 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="30" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>12</v>
@@ -2170,22 +2188,22 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="13" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F41" s="26" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="G41" s="19" t="s">
         <v>12</v>
@@ -2214,16 +2232,13 @@
       <c r="J42" s="23"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="29"/>
       <c r="B43" s="19"/>
       <c r="C43" s="16"/>
       <c r="D43" s="19"/>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
-      <c r="H43" s="19">
-        <v>1</v>
-      </c>
+      <c r="H43" s="19"/>
       <c r="I43" s="23"/>
       <c r="J43" s="23"/>
     </row>
@@ -2253,7 +2268,7 @@
       </c>
       <c r="J45" s="23">
         <f>SUM(J4:J41)</f>
-        <v>53.836999999999996</v>
+        <v>54.956999999999994</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2280,7 +2295,9 @@
       <c r="I47" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J47" s="14"/>
+      <c r="J47" s="32">
+        <v>31</v>
+      </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="19"/>
@@ -2294,75 +2311,72 @@
       <c r="I48" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J48" s="14"/>
+      <c r="J48" s="32">
+        <f>SUM(H4:H41)</f>
+        <v>63</v>
+      </c>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J49" s="14"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="J49" s="3"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="31" t="s">
+        <v>154</v>
+      </c>
       <c r="C50" s="4"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="1:12">
-      <c r="C51" s="4"/>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="1:12" s="5" customFormat="1">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="9"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
+    <row r="51" spans="1:12" s="5" customFormat="1">
+      <c r="A51" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" s="7"/>
+      <c r="C51" s="9"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="J52" s="3"/>
     </row>
     <row r="53" spans="1:12">
+      <c r="B53" s="7"/>
       <c r="C53" s="4"/>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="1:12">
-      <c r="B54" s="7"/>
-      <c r="C54" s="4"/>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="55" spans="1:12" s="5" customFormat="1">
-      <c r="C55" s="8"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="L55" s="11"/>
+    <row r="54" spans="1:12" s="5" customFormat="1">
+      <c r="C54" s="8"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="L54" s="11"/>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="C55" s="4"/>
+      <c r="J55" s="3"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="C56" s="4"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
       <c r="J56" s="3"/>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="J57" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2372,32 +2386,32 @@
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C12" r:id="rId5"/>
     <hyperlink ref="C11" r:id="rId6"/>
-    <hyperlink ref="C13" r:id="rId7"/>
-    <hyperlink ref="C29" r:id="rId8"/>
-    <hyperlink ref="C32" r:id="rId9"/>
-    <hyperlink ref="C35" r:id="rId10"/>
-    <hyperlink ref="C19" r:id="rId11"/>
-    <hyperlink ref="C25" r:id="rId12"/>
-    <hyperlink ref="C24" r:id="rId13"/>
-    <hyperlink ref="C6" r:id="rId14"/>
-    <hyperlink ref="C8" r:id="rId15"/>
-    <hyperlink ref="C21" r:id="rId16"/>
-    <hyperlink ref="C22" r:id="rId17"/>
-    <hyperlink ref="C28" r:id="rId18"/>
-    <hyperlink ref="C31" r:id="rId19"/>
-    <hyperlink ref="C23" r:id="rId20"/>
-    <hyperlink ref="C34" r:id="rId21"/>
-    <hyperlink ref="C30" r:id="rId22"/>
-    <hyperlink ref="C20" r:id="rId23"/>
-    <hyperlink ref="C39" r:id="rId24"/>
-    <hyperlink ref="C33" r:id="rId25"/>
-    <hyperlink ref="C37" r:id="rId26"/>
-    <hyperlink ref="C9" r:id="rId27"/>
-    <hyperlink ref="C26" r:id="rId28"/>
-    <hyperlink ref="C15" r:id="rId29"/>
-    <hyperlink ref="C17" r:id="rId30"/>
-    <hyperlink ref="C16" r:id="rId31"/>
-    <hyperlink ref="C41" r:id="rId32"/>
+    <hyperlink ref="C29" r:id="rId7"/>
+    <hyperlink ref="C32" r:id="rId8"/>
+    <hyperlink ref="C35" r:id="rId9"/>
+    <hyperlink ref="C25" r:id="rId10"/>
+    <hyperlink ref="C24" r:id="rId11"/>
+    <hyperlink ref="C6" r:id="rId12"/>
+    <hyperlink ref="C8" r:id="rId13"/>
+    <hyperlink ref="C21" r:id="rId14"/>
+    <hyperlink ref="C22" r:id="rId15"/>
+    <hyperlink ref="C28" r:id="rId16"/>
+    <hyperlink ref="C31" r:id="rId17"/>
+    <hyperlink ref="C23" r:id="rId18"/>
+    <hyperlink ref="C34" r:id="rId19"/>
+    <hyperlink ref="C30" r:id="rId20"/>
+    <hyperlink ref="C20" r:id="rId21"/>
+    <hyperlink ref="C39" r:id="rId22"/>
+    <hyperlink ref="C33" r:id="rId23"/>
+    <hyperlink ref="C37" r:id="rId24"/>
+    <hyperlink ref="C9" r:id="rId25"/>
+    <hyperlink ref="C26" r:id="rId26"/>
+    <hyperlink ref="C15" r:id="rId27"/>
+    <hyperlink ref="C17" r:id="rId28"/>
+    <hyperlink ref="C16" r:id="rId29"/>
+    <hyperlink ref="C41" r:id="rId30"/>
+    <hyperlink ref="C19" r:id="rId31"/>
+    <hyperlink ref="C13" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId33"/>

</xml_diff>

<commit_message>
added 47uF cap to battery
</commit_message>
<xml_diff>
--- a/doc/ecg_bom_logic_board.xlsx
+++ b/doc/ecg_bom_logic_board.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="161">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -490,6 +490,18 @@
   </si>
   <si>
     <t>Beat v1.1</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>445-5987-1-ND</t>
+  </si>
+  <si>
+    <t>C2012X5R0J476M125AC</t>
+  </si>
+  <si>
+    <t>CAP CER 47UF 6.3V 20% X5R 0805</t>
   </si>
 </sst>
 </file>
@@ -1032,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1704,7 +1716,7 @@
         <v>0.78</v>
       </c>
       <c r="J23" s="23">
-        <f t="shared" ref="J23:J37" si="1">H23*I23</f>
+        <f t="shared" ref="J23:J38" si="1">H23*I23</f>
         <v>0.78</v>
       </c>
     </row>
@@ -1809,167 +1821,167 @@
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="30"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
+      <c r="A27" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="13">
+        <v>1</v>
+      </c>
+      <c r="I27" s="23">
+        <v>0.92</v>
+      </c>
+      <c r="J27" s="23">
+        <f t="shared" si="1"/>
+        <v>0.92</v>
+      </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="30"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="25" t="s">
+      <c r="B29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D29" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E29" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F29" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="G28" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="13">
+      <c r="G29" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="13">
         <v>4</v>
       </c>
-      <c r="I28" s="23">
+      <c r="I29" s="23">
         <v>0.11</v>
       </c>
-      <c r="J28" s="23">
+      <c r="J29" s="23">
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="30" t="s">
+    <row r="30" spans="1:12">
+      <c r="A30" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="25" t="s">
+      <c r="B30" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D30" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E30" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F30" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="13">
+      <c r="G30" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="13">
         <v>1</v>
       </c>
-      <c r="I29" s="23">
+      <c r="I30" s="23">
         <v>0.13</v>
       </c>
-      <c r="J29" s="23">
+      <c r="J30" s="23">
         <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="30" t="s">
+    <row r="31" spans="1:12">
+      <c r="A31" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="25" t="s">
+      <c r="B31" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D31" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E31" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F31" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="G30" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="13">
+      <c r="G31" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="13">
         <v>1</v>
       </c>
-      <c r="I30" s="23">
+      <c r="I31" s="23">
         <v>0.12</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J31" s="23">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="19">
-        <v>1</v>
-      </c>
-      <c r="I31" s="23">
-        <v>0.13</v>
-      </c>
-      <c r="J31" s="23">
-        <f t="shared" si="1"/>
-        <v>0.13</v>
-      </c>
-    </row>
     <row r="32" spans="1:12">
       <c r="A32" s="30" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>55</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G32" s="19" t="s">
         <v>12</v>
@@ -1987,253 +1999,275 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="30" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>121</v>
+      <c r="E33" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>65</v>
       </c>
       <c r="G33" s="19" t="s">
         <v>12</v>
       </c>
       <c r="H33" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I33" s="23">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="J33" s="23">
         <f t="shared" si="1"/>
-        <v>0.33</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="30" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34" s="26" t="s">
-        <v>90</v>
+      <c r="E34" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>121</v>
       </c>
       <c r="G34" s="19" t="s">
         <v>12</v>
       </c>
       <c r="H34" s="19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I34" s="23">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="J34" s="23">
         <f t="shared" si="1"/>
-        <v>0.52</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="30" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>55</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="G35" s="19" t="s">
         <v>12</v>
       </c>
       <c r="H35" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I35" s="23">
         <v>0.13</v>
       </c>
       <c r="J35" s="23">
         <f t="shared" si="1"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="19">
+        <v>2</v>
+      </c>
+      <c r="I36" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="J36" s="23">
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="30"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-    </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="30"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="25" t="s">
+      <c r="B38" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D38" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E38" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F38" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="G37" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="19">
+      <c r="G38" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="19">
         <v>1</v>
       </c>
-      <c r="I37" s="23">
+      <c r="I38" s="23">
         <v>0.94</v>
       </c>
-      <c r="J37" s="23">
+      <c r="J38" s="23">
         <f t="shared" si="1"/>
         <v>0.94</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="30"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-    </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="30"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="25" t="s">
+      <c r="B40" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D40" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E40" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="F40" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="G39" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="13">
+      <c r="G40" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" s="13">
         <v>1</v>
       </c>
-      <c r="I39" s="23">
+      <c r="I40" s="23">
         <v>1.2</v>
       </c>
-      <c r="J39" s="23">
-        <f t="shared" ref="J39:J41" si="2">H39*I39</f>
+      <c r="J40" s="23">
+        <f t="shared" ref="J40:J42" si="2">H40*I40</f>
         <v>1.2</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="13"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="23"/>
-    </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="13"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="30" t="s">
+      <c r="B42" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D42" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E42" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="F41" s="26" t="s">
+      <c r="F42" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="G41" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="19">
+      <c r="G42" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" s="19">
         <v>4</v>
       </c>
-      <c r="I41" s="23">
+      <c r="I42" s="23">
         <v>0.6</v>
       </c>
-      <c r="J41" s="23">
+      <c r="J42" s="23">
         <f t="shared" si="2"/>
         <v>2.4</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="5" customFormat="1">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-    </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" s="5" customFormat="1">
+      <c r="A43" s="19"/>
       <c r="B43" s="19"/>
-      <c r="C43" s="16"/>
+      <c r="C43" s="21"/>
       <c r="D43" s="19"/>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
@@ -2243,7 +2277,6 @@
       <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="29"/>
       <c r="B44" s="19"/>
       <c r="C44" s="16"/>
       <c r="D44" s="19"/>
@@ -2263,28 +2296,28 @@
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
       <c r="H45" s="19"/>
-      <c r="I45" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J45" s="23">
-        <f>SUM(J4:J41)</f>
-        <v>54.956999999999994</v>
-      </c>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="22"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="19"/>
       <c r="C46" s="16"/>
       <c r="D46" s="19"/>
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46" s="23">
+        <f>SUM(J4:J42)</f>
+        <v>55.876999999999995</v>
+      </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="19"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="19"/>
       <c r="C47" s="16"/>
       <c r="D47" s="19"/>
@@ -2292,12 +2325,8 @@
       <c r="F47" s="19"/>
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
-      <c r="I47" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" s="32">
-        <v>31</v>
-      </c>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="19"/>
@@ -2309,74 +2338,90 @@
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
       <c r="I48" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" s="32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J48" s="32">
-        <f>SUM(H4:H41)</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="J49" s="3"/>
+      <c r="J49" s="32">
+        <f>SUM(H4:H42)</f>
+        <v>64</v>
+      </c>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="1:12" s="5" customFormat="1">
-      <c r="A51" s="29" t="s">
+      <c r="C51" s="4"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:12" s="5" customFormat="1">
+      <c r="A52" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="9"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-    </row>
-    <row r="52" spans="1:12">
-      <c r="A52" s="13" t="s">
+      <c r="B52" s="7"/>
+      <c r="C52" s="9"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C52" s="4"/>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="B53" s="7"/>
       <c r="C53" s="4"/>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="1:12" s="5" customFormat="1">
-      <c r="C54" s="8"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-      <c r="L54" s="11"/>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="C55" s="4"/>
-      <c r="J55" s="3"/>
+    <row r="54" spans="1:12">
+      <c r="B54" s="7"/>
+      <c r="C54" s="4"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:12" s="5" customFormat="1">
+      <c r="C55" s="8"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="L55" s="11"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
+      <c r="C56" s="4"/>
       <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="J57" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2386,35 +2431,36 @@
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C12" r:id="rId5"/>
     <hyperlink ref="C11" r:id="rId6"/>
-    <hyperlink ref="C29" r:id="rId7"/>
-    <hyperlink ref="C32" r:id="rId8"/>
-    <hyperlink ref="C35" r:id="rId9"/>
+    <hyperlink ref="C30" r:id="rId7"/>
+    <hyperlink ref="C33" r:id="rId8"/>
+    <hyperlink ref="C36" r:id="rId9"/>
     <hyperlink ref="C25" r:id="rId10"/>
     <hyperlink ref="C24" r:id="rId11"/>
     <hyperlink ref="C6" r:id="rId12"/>
     <hyperlink ref="C8" r:id="rId13"/>
     <hyperlink ref="C21" r:id="rId14"/>
     <hyperlink ref="C22" r:id="rId15"/>
-    <hyperlink ref="C28" r:id="rId16"/>
-    <hyperlink ref="C31" r:id="rId17"/>
+    <hyperlink ref="C29" r:id="rId16"/>
+    <hyperlink ref="C32" r:id="rId17"/>
     <hyperlink ref="C23" r:id="rId18"/>
-    <hyperlink ref="C34" r:id="rId19"/>
-    <hyperlink ref="C30" r:id="rId20"/>
+    <hyperlink ref="C35" r:id="rId19"/>
+    <hyperlink ref="C31" r:id="rId20"/>
     <hyperlink ref="C20" r:id="rId21"/>
-    <hyperlink ref="C39" r:id="rId22"/>
-    <hyperlink ref="C33" r:id="rId23"/>
-    <hyperlink ref="C37" r:id="rId24"/>
+    <hyperlink ref="C40" r:id="rId22"/>
+    <hyperlink ref="C34" r:id="rId23"/>
+    <hyperlink ref="C38" r:id="rId24"/>
     <hyperlink ref="C9" r:id="rId25"/>
     <hyperlink ref="C26" r:id="rId26"/>
     <hyperlink ref="C15" r:id="rId27"/>
     <hyperlink ref="C17" r:id="rId28"/>
     <hyperlink ref="C16" r:id="rId29"/>
-    <hyperlink ref="C41" r:id="rId30"/>
+    <hyperlink ref="C42" r:id="rId30"/>
     <hyperlink ref="C19" r:id="rId31"/>
     <hyperlink ref="C13" r:id="rId32"/>
+    <hyperlink ref="C27" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId33"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId34"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
removed unused scheamtic trace, updated BOM
</commit_message>
<xml_diff>
--- a/doc/ecg_bom_logic_board.xlsx
+++ b/doc/ecg_bom_logic_board.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14520"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -486,9 +486,6 @@
     <t>DO NOT PLACE</t>
   </si>
   <si>
-    <t>P1,P2,P3,P4,P6,P7</t>
-  </si>
-  <si>
     <t>Beat v1.1</t>
   </si>
   <si>
@@ -502,6 +499,9 @@
   </si>
   <si>
     <t>CAP CER 47UF 6.3V 20% X5R 0805</t>
+  </si>
+  <si>
+    <t>P1,P2,P3,P4,P5,P6,P7</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1047,7 @@
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1067,7 +1067,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1822,22 +1822,22 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="25" t="s">
         <v>157</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>158</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>47</v>
       </c>
       <c r="E27" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="F27" s="28" t="s">
         <v>159</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>160</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>12</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="13" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C53" s="4"/>
       <c r="J53" s="3"/>

</xml_diff>

<commit_message>
added lithium battery to BOM
</commit_message>
<xml_diff>
--- a/doc/ecg_bom_logic_board.xlsx
+++ b/doc/ecg_bom_logic_board.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="169">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -502,6 +502,30 @@
   </si>
   <si>
     <t>P1,P2,P3,P4,P5,P6,P7</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>BATTERY</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>PRT-00731</t>
+  </si>
+  <si>
+    <t>Great Power</t>
+  </si>
+  <si>
+    <t>GSP061225D2C</t>
+  </si>
+  <si>
+    <t>Polymer Lithium Ion Battery - 110mAh</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -694,13 +718,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -727,6 +747,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1044,16 +1070,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" bestFit="1" customWidth="1"/>
@@ -1076,7 +1102,7 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="23"/>
+      <c r="I1" s="21"/>
       <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10">
@@ -1088,7 +1114,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
-      <c r="I2" s="23"/>
+      <c r="I2" s="21"/>
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1">
@@ -1116,7 +1142,7 @@
       <c r="H3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="22" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="12" t="s">
@@ -1124,22 +1150,22 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="23" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>28</v>
       </c>
       <c r="G4" s="13" t="s">
@@ -1148,28 +1174,28 @@
       <c r="H4" s="13">
         <v>1</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="21">
         <v>14.58</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="21">
         <f>H4*I4</f>
         <v>14.58</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="13" t="s">
@@ -1181,31 +1207,31 @@
       <c r="H5" s="13">
         <v>1</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="21">
         <v>2.67</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="21">
         <f t="shared" ref="J5:J21" si="0">H5*I5</f>
         <v>2.67</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="28" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="23" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="24" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="13" t="s">
@@ -1214,16 +1240,16 @@
       <c r="H6" s="13">
         <v>1</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="21">
         <v>0.74</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="21">
         <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -1247,31 +1273,31 @@
       <c r="H7" s="13">
         <v>1</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="21">
         <v>7.56</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="21">
         <f t="shared" si="0"/>
         <v>7.56</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="28" t="s">
         <v>111</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>75</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="24" t="s">
         <v>78</v>
       </c>
       <c r="G8" s="13" t="s">
@@ -1280,31 +1306,31 @@
       <c r="H8" s="13">
         <v>3</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="21">
         <v>0.75</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="21">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="28" t="s">
         <v>112</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>113</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="24" t="s">
         <v>116</v>
       </c>
       <c r="G9" s="13" t="s">
@@ -1313,16 +1339,16 @@
       <c r="H9" s="13">
         <v>1</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="21">
         <v>0.41</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="21">
         <f t="shared" si="0"/>
         <v>0.41</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="30"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="13"/>
       <c r="C10" s="16"/>
       <c r="D10" s="13"/>
@@ -1330,26 +1356,26 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="28" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="23" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="24" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="13" t="s">
@@ -1358,16 +1384,16 @@
       <c r="H11" s="13">
         <v>1</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="21">
         <v>1.8</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="21">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -1382,7 +1408,7 @@
       <c r="E12" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="24" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="17" t="s">
@@ -1391,31 +1417,31 @@
       <c r="H12" s="13">
         <v>1</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="21">
         <v>1.2</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="21">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="28" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="23" t="s">
         <v>150</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="24" t="s">
         <v>152</v>
       </c>
       <c r="G13" s="17" t="s">
@@ -1424,43 +1450,43 @@
       <c r="H13" s="13">
         <v>1</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="21">
         <v>1.78</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J13" s="21">
         <f t="shared" si="0"/>
         <v>1.78</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="30"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="17"/>
-      <c r="C14" s="25"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="17"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="17"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="28" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="28" t="s">
         <v>133</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="24" t="s">
         <v>135</v>
       </c>
       <c r="G15" s="17" t="s">
@@ -1469,31 +1495,31 @@
       <c r="H15" s="13">
         <v>1</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="21">
         <v>1.29</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J15" s="21">
         <f t="shared" si="0"/>
         <v>1.29</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="28" t="s">
         <v>138</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="24" t="s">
         <v>140</v>
       </c>
       <c r="G16" s="17" t="s">
@@ -1502,31 +1528,31 @@
       <c r="H16" s="13">
         <v>1</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="21">
         <v>3.71</v>
       </c>
-      <c r="J16" s="23">
+      <c r="J16" s="21">
         <f t="shared" si="0"/>
         <v>3.71</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="28" t="s">
         <v>101</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="28" t="s">
         <v>136</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="24" t="s">
         <v>141</v>
       </c>
       <c r="G17" s="17" t="s">
@@ -1535,43 +1561,43 @@
       <c r="H17" s="13">
         <v>1</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="21">
         <v>4.8600000000000003</v>
       </c>
-      <c r="J17" s="23">
+      <c r="J17" s="21">
         <f>H17*I17</f>
         <v>4.8600000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="30"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="13"/>
-      <c r="C18" s="25"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="23" t="s">
         <v>147</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="24" t="s">
         <v>149</v>
       </c>
       <c r="G19" s="17" t="s">
@@ -1580,31 +1606,31 @@
       <c r="H19" s="13">
         <v>2</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="21">
         <v>0.23</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J19" s="21">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="28" t="s">
         <v>103</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="23" t="s">
         <v>84</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="25" t="s">
         <v>86</v>
       </c>
       <c r="G20" s="13" t="s">
@@ -1613,31 +1639,31 @@
       <c r="H20" s="13">
         <v>2</v>
       </c>
-      <c r="I20" s="23">
+      <c r="I20" s="21">
         <v>0.11</v>
       </c>
-      <c r="J20" s="23">
+      <c r="J20" s="21">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="28" t="s">
         <v>106</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="23" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="24" t="s">
         <v>50</v>
       </c>
       <c r="G21" s="13" t="s">
@@ -1646,31 +1672,31 @@
       <c r="H21" s="13">
         <v>5</v>
       </c>
-      <c r="I21" s="23">
+      <c r="I21" s="21">
         <v>0.41</v>
       </c>
-      <c r="J21" s="23">
+      <c r="J21" s="21">
         <f t="shared" si="0"/>
         <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="28" t="s">
         <v>105</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="23" t="s">
         <v>81</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="24" t="s">
         <v>83</v>
       </c>
       <c r="G22" s="13" t="s">
@@ -1679,31 +1705,31 @@
       <c r="H22" s="13">
         <v>11</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="21">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="21">
         <f>H22*I22</f>
         <v>0.40699999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="28" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="23" t="s">
         <v>93</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="24" t="s">
         <v>96</v>
       </c>
       <c r="G23" s="13" t="s">
@@ -1712,31 +1738,31 @@
       <c r="H23" s="13">
         <v>1</v>
       </c>
-      <c r="I23" s="23">
+      <c r="I23" s="21">
         <v>0.78</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23" s="21">
         <f t="shared" ref="J23:J38" si="1">H23*I23</f>
         <v>0.78</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="5" customFormat="1">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="28" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="23" t="s">
         <v>69</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="24" t="s">
         <v>72</v>
       </c>
       <c r="G24" s="13" t="s">
@@ -1745,32 +1771,32 @@
       <c r="H24" s="18">
         <v>2</v>
       </c>
-      <c r="I24" s="23">
+      <c r="I24" s="21">
         <v>0.42</v>
       </c>
-      <c r="J24" s="23">
+      <c r="J24" s="21">
         <f t="shared" si="1"/>
         <v>0.84</v>
       </c>
       <c r="L24" s="11"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="28" t="s">
         <v>54</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="23" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="24" t="s">
         <v>52</v>
       </c>
       <c r="G25" s="13" t="s">
@@ -1779,31 +1805,31 @@
       <c r="H25" s="13">
         <v>2</v>
       </c>
-      <c r="I25" s="23">
+      <c r="I25" s="21">
         <v>0.23</v>
       </c>
-      <c r="J25" s="23">
+      <c r="J25" s="21">
         <f t="shared" si="1"/>
         <v>0.46</v>
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="28" t="s">
         <v>107</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="23" t="s">
         <v>108</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="26" t="s">
         <v>110</v>
       </c>
       <c r="G26" s="13" t="s">
@@ -1812,31 +1838,31 @@
       <c r="H26" s="13">
         <v>1</v>
       </c>
-      <c r="I26" s="23">
+      <c r="I26" s="21">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J26" s="23">
+      <c r="J26" s="21">
         <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="28" t="s">
         <v>156</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="23" t="s">
         <v>157</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="26" t="s">
         <v>159</v>
       </c>
       <c r="G27" s="13" t="s">
@@ -1845,43 +1871,43 @@
       <c r="H27" s="13">
         <v>1</v>
       </c>
-      <c r="I27" s="23">
+      <c r="I27" s="21">
         <v>0.92</v>
       </c>
-      <c r="J27" s="23">
+      <c r="J27" s="21">
         <f t="shared" si="1"/>
         <v>0.92</v>
       </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="30"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="13"/>
-      <c r="C28" s="25"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="28" t="s">
         <v>117</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="23" t="s">
         <v>87</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="24" t="s">
         <v>89</v>
       </c>
       <c r="G29" s="13" t="s">
@@ -1890,31 +1916,31 @@
       <c r="H29" s="13">
         <v>4</v>
       </c>
-      <c r="I29" s="23">
+      <c r="I29" s="21">
         <v>0.11</v>
       </c>
-      <c r="J29" s="23">
+      <c r="J29" s="21">
         <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="28" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="23" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="24" t="s">
         <v>59</v>
       </c>
       <c r="G30" s="13" t="s">
@@ -1923,31 +1949,31 @@
       <c r="H30" s="13">
         <v>1</v>
       </c>
-      <c r="I30" s="23">
+      <c r="I30" s="21">
         <v>0.13</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J30" s="21">
         <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="28" t="s">
         <v>97</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="23" t="s">
         <v>98</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="24" t="s">
         <v>100</v>
       </c>
       <c r="G31" s="13" t="s">
@@ -1956,31 +1982,31 @@
       <c r="H31" s="13">
         <v>1</v>
       </c>
-      <c r="I31" s="23">
+      <c r="I31" s="21">
         <v>0.12</v>
       </c>
-      <c r="J31" s="23">
+      <c r="J31" s="21">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="28" t="s">
         <v>104</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="26" t="s">
+      <c r="F32" s="24" t="s">
         <v>63</v>
       </c>
       <c r="G32" s="19" t="s">
@@ -1989,31 +2015,31 @@
       <c r="H32" s="19">
         <v>1</v>
       </c>
-      <c r="I32" s="23">
+      <c r="I32" s="21">
         <v>0.13</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="21">
         <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="28" t="s">
         <v>60</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="23" t="s">
         <v>61</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="24" t="s">
         <v>65</v>
       </c>
       <c r="G33" s="19" t="s">
@@ -2022,31 +2048,31 @@
       <c r="H33" s="19">
         <v>1</v>
       </c>
-      <c r="I33" s="23">
+      <c r="I33" s="21">
         <v>0.13</v>
       </c>
-      <c r="J33" s="23">
+      <c r="J33" s="21">
         <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="28" t="s">
         <v>118</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="23" t="s">
         <v>119</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="E34" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="F34" s="27" t="s">
+      <c r="F34" s="25" t="s">
         <v>121</v>
       </c>
       <c r="G34" s="19" t="s">
@@ -2055,31 +2081,31 @@
       <c r="H34" s="19">
         <v>3</v>
       </c>
-      <c r="I34" s="23">
+      <c r="I34" s="21">
         <v>0.11</v>
       </c>
-      <c r="J34" s="23">
+      <c r="J34" s="21">
         <f t="shared" si="1"/>
         <v>0.33</v>
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="28" t="s">
         <v>123</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="23" t="s">
         <v>92</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="F35" s="26" t="s">
+      <c r="F35" s="24" t="s">
         <v>90</v>
       </c>
       <c r="G35" s="19" t="s">
@@ -2088,31 +2114,31 @@
       <c r="H35" s="19">
         <v>4</v>
       </c>
-      <c r="I35" s="23">
+      <c r="I35" s="21">
         <v>0.13</v>
       </c>
-      <c r="J35" s="23">
+      <c r="J35" s="21">
         <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="28" t="s">
         <v>80</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="23" t="s">
         <v>66</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="26" t="s">
+      <c r="E36" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="24" t="s">
         <v>67</v>
       </c>
       <c r="G36" s="19" t="s">
@@ -2121,43 +2147,43 @@
       <c r="H36" s="19">
         <v>2</v>
       </c>
-      <c r="I36" s="23">
+      <c r="I36" s="21">
         <v>0.13</v>
       </c>
-      <c r="J36" s="23">
+      <c r="J36" s="21">
         <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="30"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="19"/>
-      <c r="C37" s="25"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="13"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="28" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="23" t="s">
         <v>130</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="E38" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="F38" s="24" t="s">
         <v>132</v>
       </c>
       <c r="G38" s="19" t="s">
@@ -2166,43 +2192,43 @@
       <c r="H38" s="19">
         <v>1</v>
       </c>
-      <c r="I38" s="23">
+      <c r="I38" s="21">
         <v>0.94</v>
       </c>
-      <c r="J38" s="23">
+      <c r="J38" s="21">
         <f t="shared" si="1"/>
         <v>0.94</v>
       </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="30"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="19"/>
-      <c r="C39" s="25"/>
+      <c r="C39" s="23"/>
       <c r="D39" s="13"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="28" t="s">
         <v>124</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="23" t="s">
         <v>125</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="F40" s="26" t="s">
+      <c r="F40" s="24" t="s">
         <v>128</v>
       </c>
       <c r="G40" s="13" t="s">
@@ -2211,10 +2237,10 @@
       <c r="H40" s="13">
         <v>1</v>
       </c>
-      <c r="I40" s="23">
+      <c r="I40" s="21">
         <v>1.2</v>
       </c>
-      <c r="J40" s="23">
+      <c r="J40" s="21">
         <f t="shared" ref="J40:J42" si="2">H40*I40</f>
         <v>1.2</v>
       </c>
@@ -2222,14 +2248,14 @@
     <row r="41" spans="1:10">
       <c r="A41" s="13"/>
       <c r="B41" s="19"/>
-      <c r="C41" s="25"/>
+      <c r="C41" s="23"/>
       <c r="D41" s="13"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
       <c r="G41" s="19"/>
       <c r="H41" s="19"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="13" t="s">
@@ -2238,16 +2264,16 @@
       <c r="B42" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="28" t="s">
         <v>143</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="E42" s="26" t="s">
+      <c r="E42" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="F42" s="26" t="s">
+      <c r="F42" s="24" t="s">
         <v>146</v>
       </c>
       <c r="G42" s="19" t="s">
@@ -2256,10 +2282,10 @@
       <c r="H42" s="19">
         <v>4</v>
       </c>
-      <c r="I42" s="23">
+      <c r="I42" s="21">
         <v>0.6</v>
       </c>
-      <c r="J42" s="23">
+      <c r="J42" s="21">
         <f t="shared" si="2"/>
         <v>2.4</v>
       </c>
@@ -2267,161 +2293,143 @@
     <row r="43" spans="1:10" s="5" customFormat="1">
       <c r="A43" s="19"/>
       <c r="B43" s="19"/>
-      <c r="C43" s="21"/>
+      <c r="C43" s="20"/>
       <c r="D43" s="19"/>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
       <c r="H43" s="19"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+    </row>
+    <row r="44" spans="1:10" s="13" customFormat="1">
+      <c r="A44" s="31" t="s">
+        <v>161</v>
+      </c>
       <c r="B44" s="19"/>
       <c r="C44" s="16"/>
       <c r="D44" s="19"/>
       <c r="E44" s="19"/>
       <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="29"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+    </row>
+    <row r="45" spans="1:10" s="13" customFormat="1">
+      <c r="A45" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="H45" s="13">
+        <v>1</v>
+      </c>
+      <c r="I45" s="21">
+        <v>4.95</v>
+      </c>
+      <c r="J45" s="21">
+        <f t="shared" ref="J45" si="3">H45*I45</f>
+        <v>4.95</v>
+      </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="29"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="24" t="s">
+      <c r="A46" s="19"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:10" s="5" customFormat="1">
+      <c r="A48" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="7"/>
+      <c r="C48" s="9"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="B50" s="7"/>
+      <c r="C50" s="4"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:12" s="5" customFormat="1">
+      <c r="C51" s="8"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="J46" s="23">
+      <c r="J51" s="21">
         <f>SUM(J4:J42)</f>
         <v>55.876999999999995</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="22"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="15" t="s">
+      <c r="L51" s="11"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="C52" s="4"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J48" s="32">
+      <c r="J53" s="30">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="15" t="s">
+    <row r="54" spans="1:12">
+      <c r="I54" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J49" s="32">
+      <c r="J54" s="30">
         <f>SUM(H4:H42)</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="C51" s="4"/>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="1:12" s="5" customFormat="1">
-      <c r="A52" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="9"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C53" s="4"/>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="1:12">
-      <c r="B54" s="7"/>
-      <c r="C54" s="4"/>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="55" spans="1:12" s="5" customFormat="1">
-      <c r="C55" s="8"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="L55" s="11"/>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="C56" s="4"/>
-      <c r="J56" s="3"/>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="J57" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>